<commit_message>
support sheet names with spaces
</commit_message>
<xml_diff>
--- a/core/test/smoketest/charts.xlsx
+++ b/core/test/smoketest/charts.xlsx
@@ -7,12 +7,12 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="15120" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="data" sheetId="1" r:id="rId1"/>
+    <sheet name="data with charts" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Band">data!$A$2:$E$2</definedName>
-    <definedName name="Charts">data!$A$3:$P$43</definedName>
-    <definedName name="Header">data!$A$1:$E$1</definedName>
+    <definedName name="Band">'data with charts'!$A$2:$E$2</definedName>
+    <definedName name="Charts">'data with charts'!$A$3:$P$43</definedName>
+    <definedName name="Header">'data with charts'!$A$1:$E$1</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -192,7 +192,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$B$1</c:f>
+              <c:f>'data with charts'!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -206,7 +206,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>data!$A$2</c:f>
+              <c:f>'data with charts'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -217,7 +217,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$B$2</c:f>
+              <c:f>'data with charts'!$B$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -233,7 +233,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$C$1</c:f>
+              <c:f>'data with charts'!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -247,7 +247,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>data!$A$2</c:f>
+              <c:f>'data with charts'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -258,7 +258,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$C$2</c:f>
+              <c:f>'data with charts'!$C$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -274,7 +274,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$D$1</c:f>
+              <c:f>'data with charts'!$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -288,7 +288,7 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>data!$A$2</c:f>
+              <c:f>'data with charts'!$A$2</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -299,7 +299,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$D$2</c:f>
+              <c:f>'data with charts'!$D$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -315,7 +315,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>data!$E$1</c:f>
+              <c:f>'data with charts'!$E$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -336,7 +336,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>data!$E$2</c:f>
+              <c:f>'data with charts'!$E$2</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="1"/>
@@ -348,24 +348,24 @@
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="55363840"/>
-        <c:axId val="55377920"/>
+        <c:axId val="60548992"/>
+        <c:axId val="60550528"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="55363840"/>
+        <c:axId val="60548992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55377920"/>
+        <c:crossAx val="60550528"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="55377920"/>
+        <c:axId val="60550528"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -373,7 +373,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55363840"/>
+        <c:crossAx val="60548992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -384,8 +384,8 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.89760223359330749"/>
-          <c:y val="0.40750427935638639"/>
+          <c:x val="0.89760223359330771"/>
+          <c:y val="0.40750427935638645"/>
           <c:w val="9.4158830442341024E-2"/>
           <c:h val="0.24665525504964053"/>
         </c:manualLayout>
@@ -395,7 +395,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000422" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000422" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000433" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000433" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -414,7 +414,7 @@
           <c:order val="0"/>
           <c:cat>
             <c:strRef>
-              <c:f>data!$B$1:$D$1</c:f>
+              <c:f>'data with charts'!$B$1:$D$1</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -431,7 +431,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>data!$B$3:$D$3</c:f>
+              <c:f>'data with charts'!$B$3:$D$3</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
@@ -469,7 +469,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.750000000000001" l="0.70000000000000062" r="0.70000000000000062" t="0.750000000000001" header="0.30000000000000032" footer="0.30000000000000032"/>
+    <c:pageMargins b="0.75000000000000111" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000111" header="0.30000000000000032" footer="0.30000000000000032"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>

</xml_diff>